<commit_message>
Update lai so do
</commit_message>
<xml_diff>
--- a/2. Specification/1. Overview/DB General Schemas.xlsx
+++ b/2. Specification/1. Overview/DB General Schemas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minh_\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\GitHub\DekiruNihongo\trunk\2. Specification\1. Overview\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -44,9 +44,6 @@
     <t>Bài học</t>
   </si>
   <si>
-    <t>Từ Vựng: Mỗi ô là một cặp JSON gồm từ và nghĩa</t>
-  </si>
-  <si>
     <t>["learn", "Học"]</t>
   </si>
   <si>
@@ -84,6 +81,9 @@
   </si>
   <si>
     <t>Nếu có thời gian em sẽ code một web riêng để mn imporrt bài vào cho dễ, còn không thì imporrt thủ công cũng dc</t>
+  </si>
+  <si>
+    <t>Từ Vựng: Mỗi ô là một cặp JSON gồm từ và nghĩa, tại đầu mỗi cột có số lượng từ vựng trong cột đó</t>
   </si>
 </sst>
 </file>
@@ -145,19 +145,51 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -432,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,25 +478,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -481,56 +513,63 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -538,98 +577,118 @@
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>